<commit_message>
Add report and check status of imports
</commit_message>
<xml_diff>
--- a/data/trait-method-vocabulary+DK.xlsx
+++ b/data/trait-method-vocabulary+DK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jferrer/proyectos/fireveg/fire-veg-aust/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D542879B-DC9D-8640-AF37-3747D4B7385C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B10BADD-AC2A-6F43-8C09-EDE6D4A540F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28340" yWindow="2020" windowWidth="22880" windowHeight="12860" xr2:uid="{ED7F163C-C216-C845-81F7-32DE38F2F24D}"/>
   </bookViews>
@@ -172,12 +172,6 @@
     <t>repr3a</t>
   </si>
   <si>
-    <t>reproductive/regenerative structures not yet observed since last fire</t>
-  </si>
-  <si>
-    <t>reproductive structures observed, but uncertain whether they were also produced earlier during post-fire regeneration</t>
-  </si>
-  <si>
     <t>Inference based on relevant morphological structures or traits</t>
   </si>
   <si>
@@ -511,6 +505,12 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Reproductive structures observed, but uncertain whether they were also produced earlier during post-fire regeneration</t>
+  </si>
+  <si>
+    <t>Reproductive/regenerative structures not yet observed since last fire</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1409,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,10 +1425,10 @@
   <sheetData>
     <row r="1" spans="1:13" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>12</v>
@@ -1466,80 +1466,80 @@
     </row>
     <row r="2" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>61</v>
-      </c>
       <c r="I2" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J2" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" s="24" t="s">
+      <c r="M2" s="25" t="s">
         <v>69</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="21" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>57</v>
-      </c>
       <c r="H3" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>12</v>
@@ -1577,31 +1577,31 @@
     </row>
     <row r="5" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>22</v>
@@ -1618,16 +1618,16 @@
     </row>
     <row r="6" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>0</v>
@@ -1639,13 +1639,13 @@
         <v>20</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K6" s="27" t="s">
         <v>26</v>
@@ -1659,16 +1659,16 @@
     </row>
     <row r="7" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>0</v>
@@ -1680,13 +1680,13 @@
         <v>20</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K7" s="27" t="s">
         <v>26</v>
@@ -1706,13 +1706,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
@@ -1721,59 +1721,59 @@
         <v>21</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -1784,37 +1784,37 @@
         <v>41</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1825,34 +1825,34 @@
         <v>7</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>32</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="147" customHeight="1" x14ac:dyDescent="0.2">
@@ -1860,10 +1860,10 @@
         <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>14</v>
@@ -1878,19 +1878,19 @@
         <v>39</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>27</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>34</v>
@@ -1904,37 +1904,37 @@
         <v>4</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1945,78 +1945,78 @@
         <v>8</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>86</v>
-      </c>
       <c r="E14" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -2036,28 +2036,28 @@
         <v>2</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">

</xml_diff>